<commit_message>
FINAL TEST COMPLETE AND WORKING WITH EXCEL
</commit_message>
<xml_diff>
--- a/Results/FinalResults.xlsx
+++ b/Results/FinalResults.xlsx
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61:C71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,662 +471,449 @@
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
-        <v>6057</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>1374</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>253125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>1588</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
-        <v>262144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6">
-        <v>0.79228253760627865</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7">
-        <v>0.99460115756839906</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8">
-        <v>0.98870086669921875</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C9">
-        <v>0.81509890997174006</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C10">
-        <v>0.79771316349664056</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11">
-        <v>6532</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>2</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C12">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C13">
-        <v>251805</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C14">
-        <v>2896</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C15">
-        <v>262144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C16">
-        <v>0.69282986847687744</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C17">
-        <v>0.99639516294971431</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C18">
-        <v>0.98547744750976563</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C19">
-        <v>0.87760311702270588</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C20">
-        <v>0.7669510729406136</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C21">
-        <v>4410</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>3</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C22">
-        <v>4711</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C23">
-        <v>252000</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C24">
-        <v>1023</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C25">
-        <v>262144</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C26">
-        <v>0.81170623964660404</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C27">
-        <v>0.98164862432852507</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C28">
-        <v>0.97812652587890625</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C29">
-        <v>0.48349961627014582</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C30">
-        <v>0.59551154625844205</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C31">
-        <v>7246</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>4</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C32">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C33">
-        <v>250594</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C34">
-        <v>3353</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C35">
-        <v>262144</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C36">
-        <v>0.68364940088687609</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C37">
-        <v>0.99621936432845015</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C38">
-        <v>0.98358154296875</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C39">
-        <v>0.88398194461388313</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C40">
-        <v>0.7626447661670489</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C41">
-        <v>5434</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="11">
         <v>5</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C42">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C43">
-        <v>252739</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
       <c r="B44" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C44">
-        <v>3151</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
       <c r="B45" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C45">
-        <v>262144</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C46">
-        <v>0.63296447291788005</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C47">
-        <v>0.99676603867344482</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C48">
-        <v>0.98485183715820313</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
       <c r="B49" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C49">
-        <v>0.86888391429485134</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
       <c r="B50" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C50">
-        <v>0.72479747278606577</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
       <c r="B51" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C51">
-        <v>5200</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="11">
         <v>6</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C52">
-        <v>1190</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="11"/>
       <c r="B53" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C53">
-        <v>253538</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
       <c r="B54" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C54">
-        <v>2216</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="11"/>
       <c r="B55" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C55">
-        <v>262144</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="11"/>
       <c r="B56" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C56">
-        <v>0.70118662351672056</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="11"/>
       <c r="B57" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C57">
-        <v>0.99532835024025623</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="11"/>
       <c r="B58" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C58">
-        <v>0.98700714111328125</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
       <c r="B59" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C59">
-        <v>0.81377151799687009</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="11"/>
       <c r="B60" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C60">
-        <v>0.74666138270152604</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="11"/>
       <c r="B61" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C61">
-        <v>6949</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="11">
         <v>7</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C62">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="11"/>
       <c r="B63" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C63">
-        <v>251527</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="11"/>
       <c r="B64" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C64">
-        <v>2639</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="11"/>
       <c r="B65" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C65">
-        <v>262144</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="11"/>
       <c r="B66" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C66">
-        <v>0.72476011681268249</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="11"/>
       <c r="B67" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C67">
-        <v>0.99592565609211425</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
       <c r="B68" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C68">
-        <v>0.9860076904296875</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
       <c r="B69" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C69">
-        <v>0.87102030584106294</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="11"/>
       <c r="B70" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C70">
-        <v>0.78401173655618128</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="11"/>
       <c r="B71" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C71" t="e">
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="11">
         <v>8</v>
       </c>
@@ -1134,49 +921,49 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="11"/>
       <c r="B73" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="11"/>
       <c r="B74" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="11"/>
       <c r="B75" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="11"/>
       <c r="B76" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="11"/>
       <c r="B77" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="11"/>
       <c r="B78" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="11"/>
       <c r="B79" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="11"/>
       <c r="B80" s="3" t="s">
         <v>10</v>

</xml_diff>